<commit_message>
Added the updated LipSync Manual, LipSync Gaming User Guide, LipSync Gaming Startup Guide, and LipSync Gaming BOM File.
</commit_message>
<xml_diff>
--- a/LipSync_Gaming_BOM.xlsx
+++ b/LipSync_Gaming_BOM.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\Dropbox\Makers Making Change\Projects\LipSync\Github\LipSync-Gaming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristina Mok\Dropbox\NSS\Downloads\LipSync Files\Gaming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13153BEC-BCE2-4D7D-AA25-DE35BE7007B2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A204C7-6B66-4467-A645-48FD312A5878}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="20700" windowHeight="11140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1770" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LipSync_Gaming_BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="LipSync_BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="228">
   <si>
     <t>Qty</t>
   </si>
@@ -156,21 +156,9 @@
     <t>http://www.digikey.ca/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">1-Position Straight Female Through-Hole Header </t>
-  </si>
-  <si>
-    <t>929974-01-01</t>
-  </si>
-  <si>
     <t>3M</t>
   </si>
   <si>
-    <t>929974-01-01-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.ca/product-detail/en/3m/929974-01-01/929974-01-01-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">4-Position Straight Female Through-Hole Header  </t>
   </si>
   <si>
@@ -387,21 +375,6 @@
     <t xml:space="preserve">CAMVATE </t>
   </si>
   <si>
-    <t xml:space="preserve">Velcro Cable Tie </t>
-  </si>
-  <si>
-    <t>S0506-10-B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pearstone </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PES050610B </t>
-  </si>
-  <si>
-    <t>https://www.bhphotovideo.com/c/product/733008-REG/Pearstone_s0506_10_b_5_x_6_Touch.html</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/product-detail/en/stackpole-electronics-inc/CF14JT300R/CF14JT300RCT-ND</t>
   </si>
   <si>
@@ -604,9 +577,6 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/3m/929974-01-01/929974-01-01-ND</t>
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/keystone-electronics/25503/36-25503-ND/</t>
@@ -1597,34 +1567,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="50.453125" customWidth="1"/>
-    <col min="4" max="4" width="35.453125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="23.08984375" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" customWidth="1"/>
-    <col min="7" max="7" width="24.6328125" customWidth="1"/>
-    <col min="8" max="8" width="27.6328125" customWidth="1"/>
-    <col min="9" max="9" width="13.08984375" customWidth="1"/>
-    <col min="10" max="11" width="8.6328125" customWidth="1"/>
-    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="8.6328125" customWidth="1"/>
-    <col min="16" max="16" width="200.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.44140625" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="23.109375" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" customWidth="1"/>
+    <col min="8" max="8" width="27.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" customWidth="1"/>
+    <col min="10" max="11" width="8.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="8.6640625" customWidth="1"/>
+    <col min="16" max="16" width="200.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C1" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1633,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -1663,13 +1633,13 @@
         <v>4</v>
       </c>
       <c r="P1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="Q1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="H2" t="s">
         <v>5</v>
       </c>
@@ -1695,15 +1665,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -1712,30 +1682,30 @@
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="G3" t="s">
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="I3" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -1747,7 +1717,7 @@
         <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="G4" t="s">
         <v>21</v>
@@ -1759,79 +1729,79 @@
         <v>24</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="G5" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="H5" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D6" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="G6" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="H6" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -1843,7 +1813,7 @@
         <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="G7" t="s">
         <v>17</v>
@@ -1852,56 +1822,56 @@
         <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="P8" s="3" t="s">
         <v>33</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C9" t="s">
         <v>34</v>
@@ -1913,7 +1883,7 @@
         <v>29</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="G9" t="s">
         <v>35</v>
@@ -1922,21 +1892,21 @@
         <v>36</v>
       </c>
       <c r="I9" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
@@ -1948,254 +1918,254 @@
         <v>29</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="G10" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="H10" t="s">
         <v>30</v>
       </c>
       <c r="I10" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G11" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="G11" t="s">
-        <v>54</v>
-      </c>
       <c r="H11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" t="s">
+        <v>47</v>
+      </c>
+      <c r="P14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="G14" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" t="s">
-        <v>51</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="Q14" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="G15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
@@ -2207,7 +2177,7 @@
         <v>40</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="G18" t="s">
         <v>39</v>
@@ -2219,440 +2189,440 @@
         <v>42</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C19" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D19" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E19" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="G19" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="H19" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
-      <c r="B20" t="s">
-        <v>163</v>
+      <c r="B20" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="G20" t="s">
-        <v>44</v>
-      </c>
-      <c r="H20" t="s">
-        <v>46</v>
+        <v>214</v>
+      </c>
+      <c r="J20" t="s">
+        <v>214</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>47</v>
+        <v>215</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s">
         <v>7</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="G21" t="s">
-        <v>224</v>
+        <v>61</v>
       </c>
       <c r="J21" t="s">
-        <v>224</v>
+        <v>61</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>225</v>
+        <v>62</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" t="s">
         <v>64</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G22" t="s">
+        <v>64</v>
+      </c>
+      <c r="K22" t="s">
+        <v>64</v>
+      </c>
+      <c r="P22" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E22" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="Q22" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J22" t="s">
-        <v>65</v>
-      </c>
-      <c r="P22" s="1" t="s">
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" t="s">
         <v>66</v>
       </c>
-      <c r="Q22" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>67</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>68</v>
       </c>
-      <c r="E23" t="s">
-        <v>8</v>
-      </c>
       <c r="F23" s="2" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="G23" t="s">
-        <v>68</v>
-      </c>
-      <c r="K23" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="H23" t="s">
+        <v>69</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>69</v>
+        <v>172</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A24">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
         <v>4</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C25" t="s">
         <v>71</v>
       </c>
-      <c r="E24" t="s">
+      <c r="D25" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="G24" t="s">
-        <v>71</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="E25" t="s">
         <v>73</v>
       </c>
-      <c r="P24" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
-        <v>4</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>158</v>
-      </c>
       <c r="F25" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q25" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+        <v>208</v>
+      </c>
+      <c r="G25" t="s">
+        <v>72</v>
+      </c>
+      <c r="L25" t="s">
+        <v>72</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" t="s">
         <v>76</v>
       </c>
-      <c r="E26" t="s">
-        <v>77</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="G26" t="s">
-        <v>76</v>
-      </c>
-      <c r="L26" t="s">
-        <v>76</v>
+        <v>80</v>
+      </c>
+      <c r="H26" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26" t="s">
+        <v>193</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>236</v>
+        <v>173</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G27" t="s">
+        <v>75</v>
+      </c>
+      <c r="H27" t="s">
+        <v>77</v>
+      </c>
+      <c r="I27" t="s">
+        <v>194</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" t="s">
         <v>83</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>84</v>
       </c>
-      <c r="E27" t="s">
-        <v>80</v>
-      </c>
-      <c r="F27" s="2" t="s">
+      <c r="E28" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G28" t="s">
+        <v>84</v>
+      </c>
+      <c r="K28" t="s">
+        <v>84</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>4</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I29" t="s">
+        <v>195</v>
+      </c>
+      <c r="P29" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="G27" t="s">
-        <v>84</v>
-      </c>
-      <c r="H27" t="s">
-        <v>85</v>
-      </c>
-      <c r="I27" t="s">
-        <v>203</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q27" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>2</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C28" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" t="s">
-        <v>79</v>
-      </c>
-      <c r="E28" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="G28" t="s">
-        <v>79</v>
-      </c>
-      <c r="H28" t="s">
-        <v>81</v>
-      </c>
-      <c r="I28" t="s">
-        <v>204</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A29">
+      <c r="Q29" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="4">
+        <v>4708</v>
+      </c>
+      <c r="E30" t="s">
+        <v>200</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G30" s="4">
+        <v>4708</v>
+      </c>
+      <c r="H30" t="s">
+        <v>199</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31">
         <v>1</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C29" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" t="s">
-        <v>88</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="B31" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C31" t="s">
         <v>89</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="G29" t="s">
-        <v>88</v>
-      </c>
-      <c r="K29" t="s">
-        <v>88</v>
-      </c>
-      <c r="P29" s="1" t="s">
+      <c r="D31" t="s">
         <v>90</v>
       </c>
-      <c r="Q29" s="1" t="s">
+      <c r="E31" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G31" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2">
-        <v>4</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="I30" t="s">
-        <v>205</v>
-      </c>
-      <c r="P30" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="Q30" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>4</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="M31" t="s">
+        <v>90</v>
+      </c>
+      <c r="P31" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="4">
-        <v>4708</v>
-      </c>
-      <c r="E31" t="s">
-        <v>210</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="G31" s="4">
-        <v>4708</v>
-      </c>
-      <c r="H31" t="s">
-        <v>209</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="Q31" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C32" t="s">
         <v>93</v>
@@ -2664,285 +2634,229 @@
         <v>95</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G32" t="s">
         <v>94</v>
       </c>
-      <c r="M32" t="s">
-        <v>94</v>
+      <c r="H32" t="s">
+        <v>96</v>
+      </c>
+      <c r="I32" t="s">
+        <v>196</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C33" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D33" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E33" t="s">
+        <v>100</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G33" t="s">
         <v>99</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="G33" t="s">
-        <v>98</v>
-      </c>
-      <c r="H33" t="s">
-        <v>100</v>
-      </c>
-      <c r="I33" t="s">
-        <v>206</v>
+      <c r="N33" t="s">
+        <v>101</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="D34" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="E34" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="G34" t="s">
-        <v>103</v>
-      </c>
-      <c r="N34" t="s">
-        <v>105</v>
+        <v>114</v>
+      </c>
+      <c r="O34" t="s">
+        <v>114</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>106</v>
+        <v>198</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C35" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="D35" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="E35" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="G35" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="O35" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+      <c r="R35" t="s">
+        <v>224</v>
+      </c>
+      <c r="S35" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" t="s">
         <v>107</v>
       </c>
-      <c r="D36" t="s">
+      <c r="F36" t="s">
+        <v>208</v>
+      </c>
+      <c r="G36" t="s">
+        <v>106</v>
+      </c>
+      <c r="O36" t="s">
         <v>108</v>
       </c>
-      <c r="E36" t="s">
-        <v>109</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="G36" t="s">
-        <v>108</v>
-      </c>
-      <c r="O36" t="s">
-        <v>107</v>
-      </c>
       <c r="P36" s="1" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="R36" t="s">
-        <v>234</v>
-      </c>
-      <c r="S36" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D37" t="s">
-        <v>110</v>
+        <v>204</v>
       </c>
       <c r="E37" t="s">
-        <v>111</v>
+        <v>203</v>
       </c>
       <c r="F37" t="s">
+        <v>213</v>
+      </c>
+      <c r="G37" t="s">
+        <v>220</v>
+      </c>
+      <c r="I37" t="s">
+        <v>219</v>
+      </c>
+      <c r="P37" t="s">
         <v>218</v>
       </c>
-      <c r="G37" t="s">
-        <v>110</v>
-      </c>
-      <c r="O37" t="s">
-        <v>112</v>
-      </c>
-      <c r="P37" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q37" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="Q37" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>164</v>
+      <c r="B38" t="s">
+        <v>154</v>
       </c>
       <c r="C38" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D38" t="s">
-        <v>214</v>
+        <v>111</v>
       </c>
       <c r="E38" t="s">
-        <v>213</v>
+        <v>112</v>
       </c>
       <c r="F38" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G38" t="s">
-        <v>230</v>
-      </c>
-      <c r="I38" t="s">
-        <v>229</v>
-      </c>
-      <c r="P38" t="s">
-        <v>228</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A39">
-        <v>10</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C39" t="s">
-        <v>120</v>
-      </c>
-      <c r="D39" t="s">
-        <v>121</v>
-      </c>
-      <c r="E39" t="s">
-        <v>122</v>
-      </c>
-      <c r="F39" t="s">
-        <v>218</v>
-      </c>
-      <c r="G39" t="s">
-        <v>121</v>
-      </c>
-      <c r="N39" t="s">
-        <v>123</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q39" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
-        <v>163</v>
-      </c>
-      <c r="C40" t="s">
-        <v>114</v>
-      </c>
-      <c r="D40" t="s">
-        <v>115</v>
-      </c>
-      <c r="E40" t="s">
-        <v>116</v>
-      </c>
-      <c r="F40" t="s">
-        <v>218</v>
-      </c>
-      <c r="G40" t="s">
-        <v>115</v>
-      </c>
-      <c r="O40" t="s">
-        <v>114</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q40" s="1" t="s">
-        <v>185</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="O38" t="s">
+        <v>110</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q39" s="1"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F40" s="2"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2954,68 +2868,64 @@
     <hyperlink ref="P8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="P9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="P18" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="P20" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="P14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="P12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="P11" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="P15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="P16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="P17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="P22" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="P23" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="P24" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="P25" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="P28" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="P27" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="P29" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="P31" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="P32" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="P33" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="P34" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="P40" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="P39" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="P3" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="P4" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="P13" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="Q3" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="Q4" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="Q5" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="Q6" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="Q7" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="Q8" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="Q9" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="Q10" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="Q11" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="Q12" r:id="rId41" display="https://www.digikey.ca/product-detail/en/molex-connector-corporation/22-05-2031/WM4101-ND/" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="Q13" r:id="rId42" display="https://www.digikey.ca/product-detail/en/preci-dip/801-87-003-10-001101/1212-1180-ND" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="Q14" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="Q15" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="Q16" r:id="rId45" display="https://www.digikey.ca/product-detail/en/everlight-electronics-co-ltd/MV5437/1080-1109-ND/2675600" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="Q17" r:id="rId46" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/SPC02SYAN/S9002-ND" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="Q18" r:id="rId47" display="http://www.digikey.ca/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="Q19" r:id="rId48" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC061LFBN-RC/S7039-ND" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="Q20" r:id="rId49" display="http://www.digikey.ca/product-detail/en/3m/929974-01-01/929974-01-01-ND" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="Q22" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="Q23" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="Q24" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="Q25" r:id="rId53" display="https://www.digikey.ca/product-detail/en/essentra-components/NMS-308/RP809-ND" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="Q27" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="Q28" r:id="rId55" display="http://www.digikey.ca/product-detail/en/keystone-electronics/25503/36-25503-ND/" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="Q29" r:id="rId56" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="Q30" r:id="rId57" display="https://www.digikey.ca/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/102573" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="Q31" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="Q32" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="Q33" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="Q35" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="Q36" r:id="rId62" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="Q37" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="Q39" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="Q40" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="P35" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="P36" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="Q34" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="P26" r:id="rId69" xr:uid="{4CCDA3FE-08D0-46DF-9B30-73A601C4D5A0}"/>
-    <hyperlink ref="Q26" r:id="rId70" xr:uid="{4DAFF11F-FB4D-4481-B87D-4D729F143D51}"/>
+    <hyperlink ref="P14" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="P12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="P11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="P15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="P16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="P17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="P21" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="P22" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="P23" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="P24" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="P27" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="P26" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="P28" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="P30" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="P31" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="P32" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="P33" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="P38" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="P3" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="P4" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="P13" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="Q3" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="Q4" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="Q5" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="Q6" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="Q7" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="Q8" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="Q9" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="Q10" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="Q11" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="Q12" r:id="rId39" display="https://www.digikey.ca/product-detail/en/molex-connector-corporation/22-05-2031/WM4101-ND/" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="Q13" r:id="rId40" display="https://www.digikey.ca/product-detail/en/preci-dip/801-87-003-10-001101/1212-1180-ND" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="Q14" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="Q15" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="Q16" r:id="rId43" display="https://www.digikey.ca/product-detail/en/everlight-electronics-co-ltd/MV5437/1080-1109-ND/2675600" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="Q17" r:id="rId44" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/SPC02SYAN/S9002-ND" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="Q18" r:id="rId45" display="http://www.digikey.ca/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="Q19" r:id="rId46" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC061LFBN-RC/S7039-ND" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="Q21" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="Q22" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="Q23" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="Q24" r:id="rId50" display="https://www.digikey.ca/product-detail/en/essentra-components/NMS-308/RP809-ND" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="Q26" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="Q27" r:id="rId52" display="http://www.digikey.ca/product-detail/en/keystone-electronics/25503/36-25503-ND/" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="Q28" r:id="rId53" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="Q29" r:id="rId54" display="https://www.digikey.ca/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/102573" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="Q30" r:id="rId55" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="Q31" r:id="rId56" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="Q32" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="Q34" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="Q35" r:id="rId59" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="Q36" r:id="rId60" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="Q38" r:id="rId61" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="P34" r:id="rId62" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="P35" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="Q33" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="P25" r:id="rId65" xr:uid="{4CCDA3FE-08D0-46DF-9B30-73A601C4D5A0}"/>
+    <hyperlink ref="Q25" r:id="rId66" xr:uid="{4DAFF11F-FB4D-4481-B87D-4D729F143D51}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>